<commit_message>
adding races, removing others
</commit_message>
<xml_diff>
--- a/notebooks/terrain_data.xlsx
+++ b/notebooks/terrain_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrmik\OneDrive\Desktop\NSS\Python\Projects\Cycling_Capstone\notebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3BC6486-2B07-4142-9522-69956E1C9DC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6813D1C4-29B6-4583-AA3B-500F9F55091F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-9240" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -439,9 +439,6 @@
     <t>2023 Kuurne - Bruxelles - Kuurne</t>
   </si>
   <si>
-    <t>Kuurne-Bruxelles-Kuurne</t>
-  </si>
-  <si>
     <t>Monument, Spring, Cobbled</t>
   </si>
   <si>
@@ -470,6 +467,9 @@
   </si>
   <si>
     <t>Ronde van Vlaanderen</t>
+  </si>
+  <si>
+    <t>Kuurne-Brussel-Kuurne</t>
   </si>
 </sst>
 </file>
@@ -844,8 +844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D69" sqref="D69"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1423,7 +1423,7 @@
         <v>31</v>
       </c>
       <c r="C8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D8" t="s">
         <v>129</v>
@@ -1503,7 +1503,7 @@
         <v>32</v>
       </c>
       <c r="C9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D9" t="s">
         <v>129</v>
@@ -1583,7 +1583,7 @@
         <v>33</v>
       </c>
       <c r="C10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D10" t="s">
         <v>129</v>
@@ -1663,7 +1663,7 @@
         <v>34</v>
       </c>
       <c r="C11" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D11" t="s">
         <v>129</v>
@@ -1743,7 +1743,7 @@
         <v>35</v>
       </c>
       <c r="C12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D12" t="s">
         <v>129</v>
@@ -1823,7 +1823,7 @@
         <v>36</v>
       </c>
       <c r="C13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D13" t="s">
         <v>129</v>
@@ -1903,7 +1903,7 @@
         <v>37</v>
       </c>
       <c r="C14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D14" t="s">
         <v>129</v>
@@ -1983,10 +1983,10 @@
         <v>38</v>
       </c>
       <c r="C15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D15" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E15">
         <v>2018</v>
@@ -2063,10 +2063,10 @@
         <v>39</v>
       </c>
       <c r="C16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D16" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E16">
         <v>2019</v>
@@ -2143,10 +2143,10 @@
         <v>40</v>
       </c>
       <c r="C17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D17" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E17">
         <v>2021</v>
@@ -2223,10 +2223,10 @@
         <v>41</v>
       </c>
       <c r="C18" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E18">
         <v>2022</v>
@@ -2303,10 +2303,10 @@
         <v>42</v>
       </c>
       <c r="C19" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D19" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E19">
         <v>2023</v>
@@ -2383,10 +2383,10 @@
         <v>43</v>
       </c>
       <c r="C20" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D20" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E20">
         <v>2017</v>
@@ -2783,7 +2783,7 @@
         <v>49</v>
       </c>
       <c r="C25" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D25" t="s">
         <v>130</v>
@@ -2863,7 +2863,7 @@
         <v>50</v>
       </c>
       <c r="C26" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D26" t="s">
         <v>130</v>
@@ -2943,7 +2943,7 @@
         <v>51</v>
       </c>
       <c r="C27" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D27" t="s">
         <v>130</v>
@@ -3023,7 +3023,7 @@
         <v>52</v>
       </c>
       <c r="C28" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D28" t="s">
         <v>130</v>
@@ -3103,7 +3103,7 @@
         <v>53</v>
       </c>
       <c r="C29" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D29" t="s">
         <v>130</v>
@@ -3183,7 +3183,7 @@
         <v>54</v>
       </c>
       <c r="C30" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D30" t="s">
         <v>130</v>
@@ -3263,7 +3263,7 @@
         <v>55</v>
       </c>
       <c r="C31" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D31" t="s">
         <v>130</v>
@@ -3906,7 +3906,7 @@
         <v>65</v>
       </c>
       <c r="D39" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E39">
         <v>2017</v>
@@ -3986,7 +3986,7 @@
         <v>65</v>
       </c>
       <c r="D40" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E40">
         <v>2018</v>
@@ -4066,7 +4066,7 @@
         <v>65</v>
       </c>
       <c r="D41" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E41">
         <v>2019</v>
@@ -4146,7 +4146,7 @@
         <v>65</v>
       </c>
       <c r="D42" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E42">
         <v>2021</v>
@@ -4226,7 +4226,7 @@
         <v>65</v>
       </c>
       <c r="D43" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E43">
         <v>2022</v>
@@ -4306,7 +4306,7 @@
         <v>65</v>
       </c>
       <c r="D44" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E44">
         <v>2023</v>
@@ -4946,7 +4946,7 @@
         <v>80</v>
       </c>
       <c r="D52" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E52">
         <v>2017</v>
@@ -5026,7 +5026,7 @@
         <v>80</v>
       </c>
       <c r="D53" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E53">
         <v>2018</v>
@@ -5106,7 +5106,7 @@
         <v>80</v>
       </c>
       <c r="D54" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E54">
         <v>2019</v>
@@ -5186,7 +5186,7 @@
         <v>80</v>
       </c>
       <c r="D55" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E55">
         <v>2020</v>
@@ -5266,7 +5266,7 @@
         <v>80</v>
       </c>
       <c r="D56" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E56">
         <v>2021</v>
@@ -5346,7 +5346,7 @@
         <v>80</v>
       </c>
       <c r="D57" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E57">
         <v>2022</v>
@@ -5426,7 +5426,7 @@
         <v>80</v>
       </c>
       <c r="D58" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E58">
         <v>2023</v>
@@ -5506,7 +5506,7 @@
         <v>88</v>
       </c>
       <c r="D59" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E59">
         <v>2017</v>
@@ -5586,7 +5586,7 @@
         <v>88</v>
       </c>
       <c r="D60" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E60">
         <v>2018</v>
@@ -5666,7 +5666,7 @@
         <v>88</v>
       </c>
       <c r="D61" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E61">
         <v>2019</v>
@@ -5746,7 +5746,7 @@
         <v>88</v>
       </c>
       <c r="D62" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E62">
         <v>2021</v>
@@ -5826,7 +5826,7 @@
         <v>88</v>
       </c>
       <c r="D63" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E63">
         <v>2022</v>
@@ -5906,7 +5906,7 @@
         <v>88</v>
       </c>
       <c r="D64" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E64">
         <v>2023</v>
@@ -6143,10 +6143,10 @@
         <v>96</v>
       </c>
       <c r="C67" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D67" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E67">
         <v>2018</v>
@@ -6223,10 +6223,10 @@
         <v>97</v>
       </c>
       <c r="C68" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D68" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E68">
         <v>2019</v>
@@ -6303,10 +6303,10 @@
         <v>98</v>
       </c>
       <c r="C69" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D69" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E69">
         <v>2020</v>
@@ -6383,10 +6383,10 @@
         <v>99</v>
       </c>
       <c r="C70" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D70" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E70">
         <v>2021</v>
@@ -6463,10 +6463,10 @@
         <v>100</v>
       </c>
       <c r="C71" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D71" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E71">
         <v>2022</v>
@@ -6543,10 +6543,10 @@
         <v>101</v>
       </c>
       <c r="C72" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D72" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E72">
         <v>2023</v>
@@ -6623,10 +6623,10 @@
         <v>102</v>
       </c>
       <c r="C73" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D73" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E73">
         <v>2017</v>
@@ -7266,7 +7266,7 @@
         <v>112</v>
       </c>
       <c r="D81" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E81">
         <v>2017</v>
@@ -7346,7 +7346,7 @@
         <v>112</v>
       </c>
       <c r="D82" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E82">
         <v>2018</v>
@@ -7426,7 +7426,7 @@
         <v>112</v>
       </c>
       <c r="D83" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E83">
         <v>2019</v>
@@ -7506,7 +7506,7 @@
         <v>112</v>
       </c>
       <c r="D84" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E84">
         <v>2020</v>
@@ -7586,7 +7586,7 @@
         <v>112</v>
       </c>
       <c r="D85" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E85">
         <v>2021</v>
@@ -7666,7 +7666,7 @@
         <v>112</v>
       </c>
       <c r="D86" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E86">
         <v>2022</v>
@@ -7746,7 +7746,7 @@
         <v>112</v>
       </c>
       <c r="D87" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E87">
         <v>2023</v>
@@ -8383,7 +8383,7 @@
         <v>132</v>
       </c>
       <c r="C95" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="D95" t="s">
         <v>130</v>
@@ -8393,6 +8393,54 @@
       </c>
       <c r="F95">
         <v>202</v>
+      </c>
+      <c r="G95">
+        <v>0</v>
+      </c>
+      <c r="H95">
+        <v>0</v>
+      </c>
+      <c r="I95">
+        <v>0</v>
+      </c>
+      <c r="J95">
+        <v>0</v>
+      </c>
+      <c r="K95">
+        <v>0</v>
+      </c>
+      <c r="L95">
+        <v>0</v>
+      </c>
+      <c r="M95">
+        <v>0</v>
+      </c>
+      <c r="N95">
+        <v>0</v>
+      </c>
+      <c r="O95">
+        <v>0</v>
+      </c>
+      <c r="P95">
+        <v>0</v>
+      </c>
+      <c r="Q95">
+        <v>0</v>
+      </c>
+      <c r="R95">
+        <v>0</v>
+      </c>
+      <c r="S95">
+        <v>0</v>
+      </c>
+      <c r="T95">
+        <v>0</v>
+      </c>
+      <c r="U95">
+        <v>0</v>
+      </c>
+      <c r="V95">
+        <v>0</v>
       </c>
       <c r="W95">
         <v>9</v>
@@ -8415,7 +8463,7 @@
         <v>133</v>
       </c>
       <c r="C96" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="D96" t="s">
         <v>130</v>
@@ -8425,6 +8473,54 @@
       </c>
       <c r="F96">
         <v>202</v>
+      </c>
+      <c r="G96">
+        <v>0</v>
+      </c>
+      <c r="H96">
+        <v>0</v>
+      </c>
+      <c r="I96">
+        <v>0</v>
+      </c>
+      <c r="J96">
+        <v>0</v>
+      </c>
+      <c r="K96">
+        <v>0</v>
+      </c>
+      <c r="L96">
+        <v>0</v>
+      </c>
+      <c r="M96">
+        <v>0</v>
+      </c>
+      <c r="N96">
+        <v>0</v>
+      </c>
+      <c r="O96">
+        <v>0</v>
+      </c>
+      <c r="P96">
+        <v>0</v>
+      </c>
+      <c r="Q96">
+        <v>0</v>
+      </c>
+      <c r="R96">
+        <v>0</v>
+      </c>
+      <c r="S96">
+        <v>0</v>
+      </c>
+      <c r="T96">
+        <v>0</v>
+      </c>
+      <c r="U96">
+        <v>0</v>
+      </c>
+      <c r="V96">
+        <v>0</v>
       </c>
       <c r="W96">
         <v>9</v>
@@ -8447,7 +8543,7 @@
         <v>134</v>
       </c>
       <c r="C97" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="D97" t="s">
         <v>130</v>
@@ -8470,9 +8566,15 @@
       <c r="J97">
         <v>133</v>
       </c>
+      <c r="K97">
+        <v>0</v>
+      </c>
       <c r="L97">
         <v>91.3</v>
       </c>
+      <c r="M97">
+        <v>0</v>
+      </c>
       <c r="N97">
         <v>16.2</v>
       </c>
@@ -8482,8 +8584,23 @@
       <c r="P97">
         <v>0.47599999999999998</v>
       </c>
+      <c r="Q97">
+        <v>0</v>
+      </c>
       <c r="R97">
         <v>0.47599999999999998</v>
+      </c>
+      <c r="S97">
+        <v>0</v>
+      </c>
+      <c r="T97">
+        <v>0</v>
+      </c>
+      <c r="U97">
+        <v>0</v>
+      </c>
+      <c r="V97">
+        <v>0</v>
       </c>
       <c r="W97">
         <v>7</v>
@@ -8506,7 +8623,7 @@
         <v>135</v>
       </c>
       <c r="C98" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="D98" t="s">
         <v>130</v>
@@ -8516,6 +8633,51 @@
       </c>
       <c r="F98">
         <v>202</v>
+      </c>
+      <c r="G98">
+        <v>0</v>
+      </c>
+      <c r="H98">
+        <v>0</v>
+      </c>
+      <c r="I98">
+        <v>0</v>
+      </c>
+      <c r="J98">
+        <v>0</v>
+      </c>
+      <c r="K98">
+        <v>0</v>
+      </c>
+      <c r="L98">
+        <v>0</v>
+      </c>
+      <c r="M98">
+        <v>0</v>
+      </c>
+      <c r="N98">
+        <v>0</v>
+      </c>
+      <c r="O98">
+        <v>0</v>
+      </c>
+      <c r="P98">
+        <v>0</v>
+      </c>
+      <c r="Q98">
+        <v>0</v>
+      </c>
+      <c r="R98">
+        <v>0</v>
+      </c>
+      <c r="S98">
+        <v>0</v>
+      </c>
+      <c r="T98">
+        <v>0</v>
+      </c>
+      <c r="U98">
+        <v>0</v>
       </c>
       <c r="V98">
         <v>9.9999999999997708</v>
@@ -8541,7 +8703,7 @@
         <v>136</v>
       </c>
       <c r="C99" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="D99" t="s">
         <v>130</v>
@@ -8551,6 +8713,51 @@
       </c>
       <c r="F99">
         <v>197</v>
+      </c>
+      <c r="G99">
+        <v>0</v>
+      </c>
+      <c r="H99">
+        <v>0</v>
+      </c>
+      <c r="I99">
+        <v>0</v>
+      </c>
+      <c r="J99">
+        <v>0</v>
+      </c>
+      <c r="K99">
+        <v>0</v>
+      </c>
+      <c r="L99">
+        <v>0</v>
+      </c>
+      <c r="M99">
+        <v>0</v>
+      </c>
+      <c r="N99">
+        <v>0</v>
+      </c>
+      <c r="O99">
+        <v>0</v>
+      </c>
+      <c r="P99">
+        <v>0</v>
+      </c>
+      <c r="Q99">
+        <v>0</v>
+      </c>
+      <c r="R99">
+        <v>0</v>
+      </c>
+      <c r="S99">
+        <v>0</v>
+      </c>
+      <c r="T99">
+        <v>0</v>
+      </c>
+      <c r="U99">
+        <v>0</v>
       </c>
       <c r="V99">
         <v>9.9999999999997708</v>
@@ -8576,7 +8783,7 @@
         <v>137</v>
       </c>
       <c r="C100" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="D100" t="s">
         <v>130</v>
@@ -8586,6 +8793,54 @@
       </c>
       <c r="F100">
         <v>195</v>
+      </c>
+      <c r="G100">
+        <v>0</v>
+      </c>
+      <c r="H100">
+        <v>0</v>
+      </c>
+      <c r="I100">
+        <v>0</v>
+      </c>
+      <c r="J100">
+        <v>0</v>
+      </c>
+      <c r="K100">
+        <v>0</v>
+      </c>
+      <c r="L100">
+        <v>0</v>
+      </c>
+      <c r="M100">
+        <v>0</v>
+      </c>
+      <c r="N100">
+        <v>0</v>
+      </c>
+      <c r="O100">
+        <v>0</v>
+      </c>
+      <c r="P100">
+        <v>0</v>
+      </c>
+      <c r="Q100">
+        <v>0</v>
+      </c>
+      <c r="R100">
+        <v>0</v>
+      </c>
+      <c r="S100">
+        <v>0</v>
+      </c>
+      <c r="T100">
+        <v>0</v>
+      </c>
+      <c r="U100">
+        <v>0</v>
+      </c>
+      <c r="V100">
+        <v>0</v>
       </c>
       <c r="W100">
         <v>8</v>
@@ -8608,7 +8863,7 @@
         <v>138</v>
       </c>
       <c r="C101" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="D101" t="s">
         <v>130</v>
@@ -8631,9 +8886,15 @@
       <c r="J101">
         <v>114</v>
       </c>
+      <c r="K101">
+        <v>0</v>
+      </c>
       <c r="L101">
         <v>65.2</v>
       </c>
+      <c r="M101">
+        <v>0</v>
+      </c>
       <c r="N101">
         <v>11.8</v>
       </c>
@@ -8643,8 +8904,23 @@
       <c r="P101">
         <v>0.39500000000000002</v>
       </c>
+      <c r="Q101">
+        <v>0</v>
+      </c>
       <c r="R101">
         <v>0.39500000000000002</v>
+      </c>
+      <c r="S101">
+        <v>0</v>
+      </c>
+      <c r="T101">
+        <v>0</v>
+      </c>
+      <c r="U101">
+        <v>0</v>
+      </c>
+      <c r="V101">
+        <v>0</v>
       </c>
       <c r="W101">
         <v>8</v>

</xml_diff>

<commit_message>
windspeed visuals locked down
</commit_message>
<xml_diff>
--- a/notebooks/terrain_data.xlsx
+++ b/notebooks/terrain_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrmik\OneDrive\Desktop\NSS\Python\Projects\Cycling_Capstone\notebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AB149F6-EBEE-455D-9875-502E0C94AE0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39DCFD4A-5A51-4073-92E7-D9F7EC1ECA4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-9240" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="162">
   <si>
     <t>PCS race entry</t>
   </si>
@@ -470,6 +470,42 @@
   </si>
   <si>
     <t>2023 strade bianche</t>
+  </si>
+  <si>
+    <t>Average Windspeed</t>
+  </si>
+  <si>
+    <t>Wind Direction</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>SSE</t>
+  </si>
+  <si>
+    <t>NE</t>
+  </si>
+  <si>
+    <t>ENE</t>
+  </si>
+  <si>
+    <t>ESE</t>
+  </si>
+  <si>
+    <t>NNW</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>SSW</t>
+  </si>
+  <si>
+    <t>NNE</t>
   </si>
 </sst>
 </file>
@@ -498,7 +534,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -521,15 +557,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -832,11 +883,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y101"/>
+  <dimension ref="A1:AA102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="O1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="S1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AD10" sqref="AD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -851,9 +902,11 @@
     <col min="18" max="18" width="18.6640625" customWidth="1"/>
     <col min="19" max="19" width="12.44140625" customWidth="1"/>
     <col min="23" max="23" width="15.21875" customWidth="1"/>
+    <col min="26" max="26" width="19.88671875" customWidth="1"/>
+    <col min="27" max="27" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -929,8 +982,14 @@
       <c r="Y1" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z1" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -1006,8 +1065,14 @@
       <c r="Y2">
         <v>3150</v>
       </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z2" s="3">
+        <v>15.733333333333301</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -1083,8 +1148,14 @@
       <c r="Y3">
         <v>3160</v>
       </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z3" s="3">
+        <v>15.8666666666666</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -1160,8 +1231,14 @@
       <c r="Y4">
         <v>3190</v>
       </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z4" s="3">
+        <v>16.466666666666601</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -1237,8 +1314,14 @@
       <c r="Y5">
         <v>2420</v>
       </c>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z5" s="3">
+        <v>13.566666666666601</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -1314,8 +1397,14 @@
       <c r="Y6">
         <v>3050</v>
       </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z6" s="3">
+        <v>13.6</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>32</v>
       </c>
@@ -1391,8 +1480,14 @@
       <c r="Y7">
         <v>2970</v>
       </c>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z7" s="3">
+        <v>13.6</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -1468,8 +1563,14 @@
       <c r="Y8">
         <v>1900</v>
       </c>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z8" s="3">
+        <v>15</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -1545,8 +1646,14 @@
       <c r="Y9">
         <v>1930</v>
       </c>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z9" s="3">
+        <v>14.7666666666666</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>37</v>
       </c>
@@ -1622,8 +1729,14 @@
       <c r="Y10">
         <v>1990</v>
       </c>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z10" s="3">
+        <v>14.5</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>38</v>
       </c>
@@ -1699,8 +1812,14 @@
       <c r="Y11">
         <v>1810</v>
       </c>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z11" s="3">
+        <v>14.7666666666666</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -1776,8 +1895,14 @@
       <c r="Y12">
         <v>1920</v>
       </c>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z12" s="3">
+        <v>16.933333333333302</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>40</v>
       </c>
@@ -1853,8 +1978,14 @@
       <c r="Y13">
         <v>1820</v>
       </c>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z13" s="3">
+        <v>16.933333333333302</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>41</v>
       </c>
@@ -1930,8 +2061,14 @@
       <c r="Y14">
         <v>1840</v>
       </c>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z14" s="3">
+        <v>16.933333333333302</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -2007,8 +2144,14 @@
       <c r="Y15">
         <v>1490</v>
       </c>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z15" s="3">
+        <v>18</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>45</v>
       </c>
@@ -2084,8 +2227,14 @@
       <c r="Y16">
         <v>1350</v>
       </c>
-    </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z16" s="3">
+        <v>15.8</v>
+      </c>
+      <c r="AA16" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>46</v>
       </c>
@@ -2161,8 +2310,14 @@
       <c r="Y17">
         <v>1290</v>
       </c>
-    </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z17" s="3">
+        <v>17</v>
+      </c>
+      <c r="AA17" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>47</v>
       </c>
@@ -2238,8 +2393,14 @@
       <c r="Y18">
         <v>1429</v>
       </c>
-    </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z18" s="3">
+        <v>17.6666666666666</v>
+      </c>
+      <c r="AA18" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>48</v>
       </c>
@@ -2315,8 +2476,14 @@
       <c r="Y19">
         <v>1590</v>
       </c>
-    </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z19" s="3">
+        <v>17.2</v>
+      </c>
+      <c r="AA19" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>49</v>
       </c>
@@ -2392,8 +2559,14 @@
       <c r="Y20">
         <v>1450</v>
       </c>
-    </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z20" s="3">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="AA20" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>50</v>
       </c>
@@ -2469,8 +2642,14 @@
       <c r="Y21">
         <v>1850</v>
       </c>
-    </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z21" s="3">
+        <v>15.133333333333301</v>
+      </c>
+      <c r="AA21" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>53</v>
       </c>
@@ -2546,8 +2725,14 @@
       <c r="Y22">
         <v>1900</v>
       </c>
-    </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z22" s="3">
+        <v>15.133333333333301</v>
+      </c>
+      <c r="AA22" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>54</v>
       </c>
@@ -2623,8 +2808,14 @@
       <c r="Y23">
         <v>1940</v>
       </c>
-    </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z23" s="3">
+        <v>15.633333333333301</v>
+      </c>
+      <c r="AA23" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>55</v>
       </c>
@@ -2700,8 +2891,14 @@
       <c r="Y24">
         <v>1970</v>
       </c>
-    </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z24" s="3">
+        <v>17.3</v>
+      </c>
+      <c r="AA24" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>56</v>
       </c>
@@ -2777,8 +2974,14 @@
       <c r="Y25">
         <v>1950</v>
       </c>
-    </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z25" s="3">
+        <v>17.066666666666599</v>
+      </c>
+      <c r="AA25" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>57</v>
       </c>
@@ -2854,8 +3057,14 @@
       <c r="Y26">
         <v>1970</v>
       </c>
-    </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z26" s="3">
+        <v>17.066666666666599</v>
+      </c>
+      <c r="AA26" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>58</v>
       </c>
@@ -2931,8 +3140,14 @@
       <c r="Y27">
         <v>1520</v>
       </c>
-    </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z27" s="3">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="AA27" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>60</v>
       </c>
@@ -3008,8 +3223,14 @@
       <c r="Y28">
         <v>1510</v>
       </c>
-    </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z28" s="3">
+        <v>16.7</v>
+      </c>
+      <c r="AA28" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>61</v>
       </c>
@@ -3085,8 +3306,14 @@
       <c r="Y29">
         <v>1490</v>
       </c>
-    </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z29" s="3">
+        <v>17.6666666666666</v>
+      </c>
+      <c r="AA29" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>62</v>
       </c>
@@ -3162,8 +3389,14 @@
       <c r="Y30">
         <v>1320</v>
       </c>
-    </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z30" s="3">
+        <v>18</v>
+      </c>
+      <c r="AA30" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>63</v>
       </c>
@@ -3239,8 +3472,14 @@
       <c r="Y31">
         <v>1370</v>
       </c>
-    </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z31" s="3">
+        <v>18.133333333333301</v>
+      </c>
+      <c r="AA31" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>64</v>
       </c>
@@ -3316,8 +3555,14 @@
       <c r="Y32">
         <v>1330</v>
       </c>
-    </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z32" s="3">
+        <v>17.6666666666666</v>
+      </c>
+      <c r="AA32" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="33" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>65</v>
       </c>
@@ -3393,8 +3638,14 @@
       <c r="Y33">
         <v>1350</v>
       </c>
-    </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z33" s="3">
+        <v>16.933333333333302</v>
+      </c>
+      <c r="AA33" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="34" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>66</v>
       </c>
@@ -3470,8 +3721,14 @@
       <c r="Y34">
         <v>3950</v>
       </c>
-    </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z34" s="3">
+        <v>2.0666666666666602</v>
+      </c>
+      <c r="AA34" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="35" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>69</v>
       </c>
@@ -3547,8 +3804,14 @@
       <c r="Y35">
         <v>3840</v>
       </c>
-    </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z35" s="3">
+        <v>2.0666666666666602</v>
+      </c>
+      <c r="AA35" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="36" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>70</v>
       </c>
@@ -3624,8 +3887,14 @@
       <c r="Y36">
         <v>3930</v>
       </c>
-    </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z36" s="3">
+        <v>2.0666666666666602</v>
+      </c>
+      <c r="AA36" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="37" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>71</v>
       </c>
@@ -3701,8 +3970,14 @@
       <c r="Y37">
         <v>3790</v>
       </c>
-    </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z37" s="3">
+        <v>2</v>
+      </c>
+      <c r="AA37" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="38" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>72</v>
       </c>
@@ -3778,8 +4053,14 @@
       <c r="Y38">
         <v>4980</v>
       </c>
-    </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z38" s="3">
+        <v>1.36666666666666</v>
+      </c>
+      <c r="AA38" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="39" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>73</v>
       </c>
@@ -3855,8 +4136,14 @@
       <c r="Y39">
         <v>5290</v>
       </c>
-    </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z39" s="3">
+        <v>4.4666666666666597</v>
+      </c>
+      <c r="AA39" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="40" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>74</v>
       </c>
@@ -3932,8 +4219,14 @@
       <c r="Y40">
         <v>5110</v>
       </c>
-    </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z40" s="3">
+        <v>1.36666666666666</v>
+      </c>
+      <c r="AA40" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="41" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>75</v>
       </c>
@@ -4009,8 +4302,14 @@
       <c r="Y41">
         <v>1460</v>
       </c>
-    </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z41" s="3">
+        <v>15.133333333333301</v>
+      </c>
+      <c r="AA41" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="42" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>77</v>
       </c>
@@ -4086,8 +4385,14 @@
       <c r="Y42">
         <v>1470</v>
       </c>
-    </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z42" s="3">
+        <v>15.733333333333301</v>
+      </c>
+      <c r="AA42" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="43" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>78</v>
       </c>
@@ -4163,8 +4468,14 @@
       <c r="Y43">
         <v>1470</v>
       </c>
-    </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z43" s="3">
+        <v>15.466666666666599</v>
+      </c>
+      <c r="AA43" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="44" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>79</v>
       </c>
@@ -4240,8 +4551,14 @@
       <c r="Y44">
         <v>1679</v>
       </c>
-    </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z44" s="3">
+        <v>15.233333333333301</v>
+      </c>
+      <c r="AA44" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="45" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>80</v>
       </c>
@@ -4317,8 +4634,14 @@
       <c r="Y45">
         <v>1679</v>
       </c>
-    </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z45" s="3">
+        <v>16.3333333333333</v>
+      </c>
+      <c r="AA45" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="46" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>81</v>
       </c>
@@ -4394,8 +4717,14 @@
       <c r="Y46">
         <v>1770</v>
       </c>
-    </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z46" s="3">
+        <v>16.8</v>
+      </c>
+      <c r="AA46" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="47" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>82</v>
       </c>
@@ -4471,8 +4800,14 @@
       <c r="Y47">
         <v>1740</v>
       </c>
-    </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z47" s="3">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="AA47" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="48" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>83</v>
       </c>
@@ -4548,8 +4883,14 @@
       <c r="Y48">
         <v>2620</v>
       </c>
-    </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z48" s="3">
+        <v>14.533333333333299</v>
+      </c>
+      <c r="AA48" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="49" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>85</v>
       </c>
@@ -4625,8 +4966,14 @@
       <c r="Y49">
         <v>3320</v>
       </c>
-    </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z49" s="3">
+        <v>14.299999999999899</v>
+      </c>
+      <c r="AA49" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="50" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>86</v>
       </c>
@@ -4702,8 +5049,14 @@
       <c r="Y50">
         <v>2840</v>
       </c>
-    </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z50" s="3">
+        <v>15.966666666666599</v>
+      </c>
+      <c r="AA50" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="51" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>87</v>
       </c>
@@ -4779,8 +5132,14 @@
       <c r="Y51">
         <v>3100</v>
       </c>
-    </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z51" s="3">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="AA51" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="52" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>88</v>
       </c>
@@ -4856,8 +5215,14 @@
       <c r="Y52">
         <v>2720</v>
       </c>
-    </row>
-    <row r="53" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z52" s="3">
+        <v>16.8</v>
+      </c>
+      <c r="AA52" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="53" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>89</v>
       </c>
@@ -4933,8 +5298,14 @@
       <c r="Y53">
         <v>3040</v>
       </c>
-    </row>
-    <row r="54" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z53" s="3">
+        <v>18.3333333333333</v>
+      </c>
+      <c r="AA53" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="54" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>90</v>
       </c>
@@ -5010,8 +5381,14 @@
       <c r="Y54">
         <v>3140</v>
       </c>
-    </row>
-    <row r="55" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z54" s="3">
+        <v>18</v>
+      </c>
+      <c r="AA54" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="55" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>91</v>
       </c>
@@ -5087,8 +5464,14 @@
       <c r="Y55">
         <v>4090</v>
       </c>
-    </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z55" s="3">
+        <v>9.93333333333333</v>
+      </c>
+      <c r="AA55" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="56" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>94</v>
       </c>
@@ -5164,8 +5547,14 @@
       <c r="Y56">
         <v>2800</v>
       </c>
-    </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z56" s="3">
+        <v>10.7666666666666</v>
+      </c>
+      <c r="AA56" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="57" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>95</v>
       </c>
@@ -5241,8 +5630,14 @@
       <c r="Y57">
         <v>2790</v>
       </c>
-    </row>
-    <row r="58" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z57" s="3">
+        <v>12.8333333333333</v>
+      </c>
+      <c r="AA57" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="58" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>96</v>
       </c>
@@ -5318,8 +5713,14 @@
       <c r="Y58">
         <v>4150</v>
       </c>
-    </row>
-    <row r="59" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z58" s="3">
+        <v>13.4333333333333</v>
+      </c>
+      <c r="AA58" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="59" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>97</v>
       </c>
@@ -5395,8 +5796,14 @@
       <c r="Y59">
         <v>4160</v>
       </c>
-    </row>
-    <row r="60" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z59" s="3">
+        <v>10.1666666666666</v>
+      </c>
+      <c r="AA59" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="60" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>98</v>
       </c>
@@ -5472,8 +5879,14 @@
       <c r="Y60">
         <v>2980</v>
       </c>
-    </row>
-    <row r="61" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z60" s="3">
+        <v>11.033333333333299</v>
+      </c>
+      <c r="AA60" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="61" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>99</v>
       </c>
@@ -5549,8 +5962,14 @@
       <c r="Y61">
         <v>2270</v>
       </c>
-    </row>
-    <row r="62" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z61" s="3">
+        <v>13.2</v>
+      </c>
+      <c r="AA61" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="62" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>101</v>
       </c>
@@ -5626,8 +6045,14 @@
       <c r="Y62">
         <v>2200</v>
       </c>
-    </row>
-    <row r="63" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z62" s="3">
+        <v>6.93333333333333</v>
+      </c>
+      <c r="AA62" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="63" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>102</v>
       </c>
@@ -5703,8 +6128,14 @@
       <c r="Y63">
         <v>2210</v>
       </c>
-    </row>
-    <row r="64" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z63" s="3">
+        <v>6.93333333333333</v>
+      </c>
+      <c r="AA63" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="64" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>103</v>
       </c>
@@ -5780,8 +6211,14 @@
       <c r="Y64">
         <v>3440</v>
       </c>
-    </row>
-    <row r="65" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z64" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="AA64" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="65" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>104</v>
       </c>
@@ -5857,8 +6294,14 @@
       <c r="Y65">
         <v>2110</v>
       </c>
-    </row>
-    <row r="66" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z65" s="3">
+        <v>4.8333333333333304</v>
+      </c>
+      <c r="AA65" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="66" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>105</v>
       </c>
@@ -5934,8 +6377,14 @@
       <c r="Y66">
         <v>2220</v>
       </c>
-    </row>
-    <row r="67" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z66" s="3">
+        <v>4.3999999999999897</v>
+      </c>
+      <c r="AA66" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="67" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>106</v>
       </c>
@@ -6011,8 +6460,14 @@
       <c r="Y67">
         <v>2300</v>
       </c>
-    </row>
-    <row r="68" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z67" s="3">
+        <v>5.7666666666666604</v>
+      </c>
+      <c r="AA67" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="68" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>107</v>
       </c>
@@ -6088,8 +6543,14 @@
       <c r="Y68">
         <v>1620</v>
       </c>
-    </row>
-    <row r="69" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z68" s="3">
+        <v>6.1333333333333302</v>
+      </c>
+      <c r="AA68" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="69" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>110</v>
       </c>
@@ -6165,8 +6626,14 @@
       <c r="Y69">
         <v>1550</v>
       </c>
-    </row>
-    <row r="70" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z69" s="3">
+        <v>16.8333333333333</v>
+      </c>
+      <c r="AA69" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="70" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>111</v>
       </c>
@@ -6242,8 +6709,14 @@
       <c r="Y70">
         <v>1560</v>
       </c>
-    </row>
-    <row r="71" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z70" s="3">
+        <v>17.033333333333299</v>
+      </c>
+      <c r="AA70" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="71" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>112</v>
       </c>
@@ -6319,8 +6792,14 @@
       <c r="Y71">
         <v>1530</v>
       </c>
-    </row>
-    <row r="72" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z71" s="3">
+        <v>17.1666666666666</v>
+      </c>
+      <c r="AA71" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="72" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>113</v>
       </c>
@@ -6396,8 +6875,14 @@
       <c r="Y72">
         <v>1580</v>
       </c>
-    </row>
-    <row r="73" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z72" s="3">
+        <v>17.1666666666666</v>
+      </c>
+      <c r="AA72" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="73" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>114</v>
       </c>
@@ -6473,8 +6958,14 @@
       <c r="Y73">
         <v>1560</v>
       </c>
-    </row>
-    <row r="74" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z73" s="3">
+        <v>18.8333333333333</v>
+      </c>
+      <c r="AA73" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="74" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>115</v>
       </c>
@@ -6550,8 +7041,14 @@
       <c r="Y74">
         <v>1550</v>
       </c>
-    </row>
-    <row r="75" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z74" s="3">
+        <v>18.133333333333301</v>
+      </c>
+      <c r="AA74" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="75" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>116</v>
       </c>
@@ -6627,8 +7124,14 @@
       <c r="Y75">
         <v>1200</v>
       </c>
-    </row>
-    <row r="76" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z75" s="3">
+        <v>18.266666666666602</v>
+      </c>
+      <c r="AA75" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="76" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>119</v>
       </c>
@@ -6704,8 +7207,14 @@
       <c r="Y76">
         <v>1220</v>
       </c>
-    </row>
-    <row r="77" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z76" s="3">
+        <v>12.8</v>
+      </c>
+      <c r="AA76" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="77" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>120</v>
       </c>
@@ -6781,8 +7290,14 @@
       <c r="Y77">
         <v>1240</v>
       </c>
-    </row>
-    <row r="78" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z77" s="3">
+        <v>13.066666666666601</v>
+      </c>
+      <c r="AA77" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="78" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>121</v>
       </c>
@@ -6858,8 +7373,14 @@
       <c r="Y78">
         <v>1220</v>
       </c>
-    </row>
-    <row r="79" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z78" s="3">
+        <v>12.8</v>
+      </c>
+      <c r="AA78" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="79" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>122</v>
       </c>
@@ -6935,8 +7456,14 @@
       <c r="Y79">
         <v>1220</v>
       </c>
-    </row>
-    <row r="80" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z79" s="3">
+        <v>16.6666666666666</v>
+      </c>
+      <c r="AA79" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="80" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>123</v>
       </c>
@@ -7012,8 +7539,14 @@
       <c r="Y80">
         <v>1250</v>
       </c>
-    </row>
-    <row r="81" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z80" s="3">
+        <v>16.6666666666666</v>
+      </c>
+      <c r="AA80" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="81" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>124</v>
       </c>
@@ -7089,8 +7622,14 @@
       <c r="Y81">
         <v>2130</v>
       </c>
-    </row>
-    <row r="82" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z81" s="3">
+        <v>16.566666666666599</v>
+      </c>
+      <c r="AA81" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="82" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>127</v>
       </c>
@@ -7166,8 +7705,14 @@
       <c r="Y82">
         <v>2170</v>
       </c>
-    </row>
-    <row r="83" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z82" s="3">
+        <v>17.266666666666602</v>
+      </c>
+      <c r="AA82" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="83" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>128</v>
       </c>
@@ -7243,8 +7788,14 @@
       <c r="Y83">
         <v>2200</v>
       </c>
-    </row>
-    <row r="84" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z83" s="3">
+        <v>17.033333333333299</v>
+      </c>
+      <c r="AA83" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="84" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>129</v>
       </c>
@@ -7320,8 +7871,14 @@
       <c r="Y84">
         <v>1990</v>
       </c>
-    </row>
-    <row r="85" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z84" s="3">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="AA84" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="85" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>130</v>
       </c>
@@ -7397,8 +7954,14 @@
       <c r="Y85">
         <v>2170</v>
       </c>
-    </row>
-    <row r="86" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z85" s="3">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="AA85" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="86" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>131</v>
       </c>
@@ -7474,8 +8037,14 @@
       <c r="Y86">
         <v>2230</v>
       </c>
-    </row>
-    <row r="87" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z86" s="3">
+        <v>17.766666666666602</v>
+      </c>
+      <c r="AA86" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="87" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>132</v>
       </c>
@@ -7551,8 +8120,14 @@
       <c r="Y87">
         <v>2190</v>
       </c>
-    </row>
-    <row r="88" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z87" s="3">
+        <v>17.533333333333299</v>
+      </c>
+      <c r="AA87" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="88" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>133</v>
       </c>
@@ -7628,8 +8203,14 @@
       <c r="Y88">
         <v>510</v>
       </c>
-    </row>
-    <row r="89" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z88" s="3">
+        <v>18.8333333333333</v>
+      </c>
+      <c r="AA88" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="89" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>135</v>
       </c>
@@ -7705,8 +8286,14 @@
       <c r="Y89">
         <v>330</v>
       </c>
-    </row>
-    <row r="90" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z89" s="3">
+        <v>13.2</v>
+      </c>
+      <c r="AA89" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="90" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>136</v>
       </c>
@@ -7782,8 +8369,14 @@
       <c r="Y90">
         <v>290</v>
       </c>
-    </row>
-    <row r="91" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z90" s="3">
+        <v>18.3666666666666</v>
+      </c>
+      <c r="AA90" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="91" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>137</v>
       </c>
@@ -7859,8 +8452,14 @@
       <c r="Y91">
         <v>370</v>
       </c>
-    </row>
-    <row r="92" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z91" s="3">
+        <v>18.3666666666666</v>
+      </c>
+      <c r="AA91" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="92" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>138</v>
       </c>
@@ -7936,8 +8535,14 @@
       <c r="Y92">
         <v>350</v>
       </c>
-    </row>
-    <row r="93" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z92" s="3">
+        <v>15.1</v>
+      </c>
+      <c r="AA92" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="93" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>139</v>
       </c>
@@ -8013,8 +8618,14 @@
       <c r="Y93">
         <v>370</v>
       </c>
-    </row>
-    <row r="94" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z93" s="3">
+        <v>15.233333333333301</v>
+      </c>
+      <c r="AA93" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="94" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>140</v>
       </c>
@@ -8090,8 +8701,14 @@
       <c r="Y94">
         <v>390</v>
       </c>
-    </row>
-    <row r="95" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z94" s="3">
+        <v>14.8666666666666</v>
+      </c>
+      <c r="AA94" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="95" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>141</v>
       </c>
@@ -8167,8 +8784,14 @@
       <c r="Y95">
         <v>2720</v>
       </c>
-    </row>
-    <row r="96" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z95" s="3">
+        <v>15.466666666666599</v>
+      </c>
+      <c r="AA95" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="96" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>144</v>
       </c>
@@ -8244,8 +8867,14 @@
       <c r="Y96">
         <v>2790</v>
       </c>
-    </row>
-    <row r="97" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z96" s="3">
+        <v>2.36666666666666</v>
+      </c>
+      <c r="AA96" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="97" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>145</v>
       </c>
@@ -8321,8 +8950,14 @@
       <c r="Y97">
         <v>2790</v>
       </c>
-    </row>
-    <row r="98" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z97" s="3">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AA97" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="98" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>146</v>
       </c>
@@ -8398,8 +9033,14 @@
       <c r="Y98">
         <v>2790</v>
       </c>
-    </row>
-    <row r="99" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z98" s="3">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AA98" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="99" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>147</v>
       </c>
@@ -8475,8 +9116,14 @@
       <c r="Y99">
         <v>2790</v>
       </c>
-    </row>
-    <row r="100" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z99" s="3">
+        <v>1.4666666666666599</v>
+      </c>
+      <c r="AA99" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="100" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>148</v>
       </c>
@@ -8552,8 +9199,14 @@
       <c r="Y100">
         <v>2790</v>
       </c>
-    </row>
-    <row r="101" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z100" s="3">
+        <v>1.7333333333333301</v>
+      </c>
+      <c r="AA100" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="101" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>149</v>
       </c>
@@ -8628,6 +9281,20 @@
       </c>
       <c r="Y101">
         <v>2890</v>
+      </c>
+      <c r="Z101" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="AA101" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="102" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="Z102" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="AA102" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>